<commit_message>
fixing conversion of units
</commit_message>
<xml_diff>
--- a/Aggregations/Aggregation_plots.xlsx
+++ b/Aggregations/Aggregation_plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8099CE03-5F8A-4085-A87C-AE3569C2E620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D872EE-E863-4AE5-8EC4-92B8420DF5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Agriculture, cattling &amp; fishering</t>
   </si>
@@ -90,6 +90,27 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>PV plants</t>
+  </si>
+  <si>
+    <t>Onshore wind plants</t>
+  </si>
+  <si>
+    <t>DFIG generators</t>
+  </si>
+  <si>
+    <t>Offshore wind plants</t>
+  </si>
+  <si>
+    <t>PMG generators</t>
+  </si>
+  <si>
+    <t>Electricity by PV</t>
+  </si>
+  <si>
+    <t>Electricity by wind</t>
   </si>
 </sst>
 </file>
@@ -416,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,23 +546,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -549,10 +570,66 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>